<commit_message>
magnific poput anf jquery new version files
</commit_message>
<xml_diff>
--- a/upload/contract/contract_ext.xlsx
+++ b/upload/contract/contract_ext.xlsx
@@ -147,13 +147,13 @@
     <t>Вартість велосипеду (грн.)</t>
   </si>
   <si>
-    <t>За перевищення часу прокату, зазначеному в цьому договорі, сплачується 10 грн. за кожну наступну годину.</t>
-  </si>
-  <si>
     <t>Адреса проживання/прописки:___________________________________________</t>
   </si>
   <si>
     <t>_______________________________________________підпис:_________________</t>
+  </si>
+  <si>
+    <t>За перевищення часу прокату, зазначеному в цьому договорі, сплачується 20 грн. за кожну наступну годину.</t>
   </si>
 </sst>
 </file>
@@ -368,10 +368,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -386,9 +389,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,8 +696,8 @@
   </sheetPr>
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -729,12 +729,12 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="16"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -744,12 +744,12 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="16"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -837,11 +837,11 @@
     </row>
     <row r="9" spans="1:11" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="19"/>
       <c r="F9" s="9">
         <f>SUM(F6:F8)</f>
@@ -870,13 +870,13 @@
       <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -887,13 +887,13 @@
       <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -902,13 +902,13 @@
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -919,13 +919,13 @@
       <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -936,13 +936,13 @@
       <c r="A15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -953,13 +953,13 @@
       <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -970,13 +970,13 @@
       <c r="A17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -985,13 +985,13 @@
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1002,13 +1002,13 @@
       <c r="A19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1019,13 +1019,13 @@
       <c r="A20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1034,13 +1034,13 @@
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1049,13 +1049,13 @@
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1066,13 +1066,13 @@
       <c r="A23" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
+      <c r="B23" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1083,13 +1083,13 @@
       <c r="A24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1100,13 +1100,13 @@
       <c r="A25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1115,13 +1115,13 @@
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1132,13 +1132,13 @@
       <c r="A27" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -1149,13 +1149,13 @@
       <c r="A28" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -1164,13 +1164,13 @@
     </row>
     <row r="29" spans="1:11" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1180,7 +1180,7 @@
     <row r="30" spans="1:11" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -1195,7 +1195,7 @@
     <row r="31" spans="1:11" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
@@ -1209,13 +1209,13 @@
     </row>
     <row r="32" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1279,31 +1279,31 @@
       <c r="A40" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C43" s="13"/>
@@ -1312,16 +1312,27 @@
       <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="25"/>
+      <c r="C44" s="24"/>
       <c r="D44" s="13"/>
       <c r="E44" s="17"/>
       <c r="F44" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B23:F23"/>
     <mergeCell ref="B42:F42"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B12:F12"/>
@@ -1338,17 +1349,6 @@
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B16:F16"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B23:F23"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.19685039370078741" top="0.74803149606299213" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="93" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changed text in contract
</commit_message>
<xml_diff>
--- a/upload/contract/contract_ext.xlsx
+++ b/upload/contract/contract_ext.xlsx
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$F$44</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>ДОГОВІР ПРО НАДАННЯ ПОСЛУГ ПРОКАТУ ВЕЛОСИПЕДА</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Велосипед видав__________________</t>
   </si>
   <si>
-    <t>Велосипед прийняв____________________</t>
-  </si>
-  <si>
     <t xml:space="preserve">Заволодіння чужим майном або придбання права на майно шляхом обману чи зловживанням </t>
   </si>
   <si>
@@ -154,6 +151,12 @@
   </si>
   <si>
     <t>За перевищення часу прокату, зазначеному в цьому договорі, сплачується 20 грн. за кожну наступну годину.</t>
+  </si>
+  <si>
+    <t>Велосипед прийняв</t>
+  </si>
+  <si>
+    <t>в повністю справному стані_________________</t>
   </si>
 </sst>
 </file>
@@ -368,27 +371,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,8 +699,8 @@
   </sheetPr>
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:F23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -729,12 +732,12 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="16"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -744,12 +747,12 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="16"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -785,10 +788,10 @@
         <v>6</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="5"/>
@@ -837,11 +840,11 @@
     </row>
     <row r="9" spans="1:11" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="19"/>
       <c r="F9" s="9">
         <f>SUM(F6:F8)</f>
@@ -870,13 +873,13 @@
       <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -887,13 +890,13 @@
       <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -902,13 +905,13 @@
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -919,13 +922,13 @@
       <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -936,13 +939,13 @@
       <c r="A15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -953,13 +956,13 @@
       <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -970,13 +973,13 @@
       <c r="A17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -985,13 +988,13 @@
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1002,13 +1005,13 @@
       <c r="A19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1019,13 +1022,13 @@
       <c r="A20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1034,13 +1037,13 @@
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1049,13 +1052,13 @@
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1066,13 +1069,13 @@
       <c r="A23" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
+      <c r="B23" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1083,13 +1086,13 @@
       <c r="A24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1100,13 +1103,13 @@
       <c r="A25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1115,13 +1118,13 @@
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1132,13 +1135,13 @@
       <c r="A27" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -1149,13 +1152,13 @@
       <c r="A28" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -1164,13 +1167,13 @@
     </row>
     <row r="29" spans="1:11" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1180,7 +1183,7 @@
     <row r="30" spans="1:11" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -1195,7 +1198,7 @@
     <row r="31" spans="1:11" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
@@ -1209,13 +1212,13 @@
     </row>
     <row r="32" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1228,7 +1231,7 @@
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="13"/>
@@ -1239,6 +1242,9 @@
       <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1279,31 +1285,31 @@
       <c r="A40" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B41" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
+      <c r="B42" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C43" s="13"/>
@@ -1312,27 +1318,16 @@
       <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B44" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="24"/>
+      <c r="B44" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="25"/>
       <c r="D44" s="13"/>
       <c r="E44" s="17"/>
       <c r="F44" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B23:F23"/>
     <mergeCell ref="B42:F42"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B12:F12"/>
@@ -1349,6 +1344,17 @@
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B16:F16"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B23:F23"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.19685039370078741" top="0.74803149606299213" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="93" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>